<commit_message>
made plots in R markdown file
</commit_message>
<xml_diff>
--- a/data/EXP 1/exp1_qPCR_results.xlsx
+++ b/data/EXP 1/exp1_qPCR_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviacattau/Documents/GitHub/fish541_lab/data/EXP 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85BDFAF3-2B77-A54C-9746-7E1B4BC5E403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7220CF49-F5CE-F443-9385-0DACBA298725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31260" yWindow="-1380" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,6 @@
     <sheet name="quant plate view " sheetId="7" r:id="rId8"/>
     <sheet name="Run Information" sheetId="2" r:id="rId9"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">exp1_qPCR_results!$D$1:$D$41</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="260">
   <si>
     <t>Well</t>
   </si>
@@ -732,15 +729,6 @@
     <t>Cq (average)</t>
   </si>
   <si>
-    <t>average Cq</t>
-  </si>
-  <si>
-    <t>Housekeeping Gene (GABB45)</t>
-  </si>
-  <si>
-    <t>Gene of Interest (HSC70)</t>
-  </si>
-  <si>
     <t>Delta Cq</t>
   </si>
   <si>
@@ -819,7 +807,19 @@
     <t>HS Treatment</t>
   </si>
   <si>
-    <t>no results/conclusions</t>
+    <t>average Cq (GABB45)</t>
+  </si>
+  <si>
+    <t>average Cq (HSC70)</t>
+  </si>
+  <si>
+    <t>Sample(2)</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>HS</t>
   </si>
 </sst>
 </file>
@@ -829,7 +829,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="###0.00;\-###0.00"/>
     <numFmt numFmtId="165" formatCode="###0;\-###0"/>
-    <numFmt numFmtId="170" formatCode="0.00_);\(0.00\)"/>
+    <numFmt numFmtId="166" formatCode="0.00_);\(0.00\)"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1206,19 +1206,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1226,7 +1214,7 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1238,7 +1226,7 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1246,7 +1234,7 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1256,6 +1244,18 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3698,11 +3698,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D366DB0-ADA9-7F47-A64B-307E5A959B55}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3714,583 +3714,634 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" t="s">
         <v>230</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="53" t="s">
         <v>231</v>
       </c>
+      <c r="H1" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>253</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="K1" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="A2" s="48">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>229</v>
-      </c>
-      <c r="E2" t="s">
-        <v>232</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B2" s="48">
+        <v>39.43</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="48">
+        <v>27.265000000000001</v>
+      </c>
+      <c r="E2" s="49">
+        <v>-12.164999999999999</v>
+      </c>
+      <c r="F2" s="44">
+        <f>E2-$G$2</f>
+        <v>-4.4099999999999984</v>
+      </c>
+      <c r="G2" s="51">
+        <f>AVERAGE(E2:E11)</f>
+        <v>-7.7550000000000008</v>
+      </c>
+      <c r="H2" s="44">
+        <f>2^-(F2)</f>
+        <v>21.258973025544162</v>
+      </c>
+      <c r="I2" s="44">
+        <f>AVERAGE(H2:H11)</f>
+        <v>6.7528000808925501</v>
+      </c>
+      <c r="J2" s="44">
+        <f>AVERAGE(H12:H21)</f>
+        <v>2.1236362321936868</v>
+      </c>
+      <c r="K2" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A3" s="48">
+        <v>11</v>
+      </c>
+      <c r="B3" s="48">
+        <v>40</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="48">
+        <v>34.085000000000001</v>
+      </c>
+      <c r="E3" s="49">
+        <f>D3-B3</f>
+        <v>-5.9149999999999991</v>
+      </c>
+      <c r="F3" s="44">
+        <f t="shared" ref="F3:F21" si="0">E3-$G$2</f>
+        <v>1.8400000000000016</v>
+      </c>
+      <c r="H3" s="44">
+        <f t="shared" ref="H3:H21" si="1">2^-(F3)</f>
+        <v>0.27932178451805473</v>
+      </c>
+      <c r="K3" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A4" s="48">
+        <v>2</v>
+      </c>
+      <c r="B4" s="48">
+        <v>37.909999999999997</v>
+      </c>
+      <c r="C4" s="48" t="s">
         <v>233</v>
       </c>
-      <c r="G2" s="56" t="s">
-        <v>234</v>
-      </c>
-      <c r="H2" s="55" t="s">
-        <v>255</v>
-      </c>
-      <c r="I2" s="55" t="s">
-        <v>256</v>
-      </c>
-      <c r="J2" s="55" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A3" s="51">
-        <v>4</v>
-      </c>
-      <c r="B3" s="51">
-        <v>39.43</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>238</v>
-      </c>
-      <c r="D3" s="51">
-        <v>27.265000000000001</v>
-      </c>
-      <c r="E3" s="52">
-        <v>-12.164999999999999</v>
-      </c>
-      <c r="F3" s="47">
-        <f>E3-$G$3</f>
-        <v>-4.4099999999999984</v>
-      </c>
-      <c r="G3" s="54">
-        <f>AVERAGE(E3:E12)</f>
-        <v>-7.7550000000000008</v>
-      </c>
-      <c r="H3" s="47">
-        <f>2^-(F3)</f>
-        <v>21.258973025544162</v>
-      </c>
-      <c r="I3" s="47">
-        <f>AVERAGE(H3:H12)</f>
-        <v>6.7528000808925501</v>
-      </c>
-      <c r="J3" s="47">
-        <f>AVERAGE(H13:H22)</f>
-        <v>2.1236362321936868</v>
-      </c>
-      <c r="K3" s="55" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A4" s="51">
-        <v>11</v>
-      </c>
-      <c r="B4" s="51">
-        <v>40</v>
-      </c>
-      <c r="C4" s="51" t="s">
-        <v>245</v>
-      </c>
-      <c r="D4" s="51">
-        <v>34.085000000000001</v>
-      </c>
-      <c r="E4" s="52">
-        <f>D4-B4</f>
-        <v>-5.9149999999999991</v>
-      </c>
-      <c r="F4" s="47">
-        <f t="shared" ref="F4:F22" si="0">E4-$G$3</f>
-        <v>1.8400000000000016</v>
-      </c>
-      <c r="H4" s="47">
-        <f t="shared" ref="H4:H22" si="1">2^-(F4)</f>
-        <v>0.27932178451805473</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A5" s="51">
-        <v>2</v>
-      </c>
-      <c r="B5" s="51">
-        <v>37.909999999999997</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>236</v>
-      </c>
-      <c r="D5" s="51">
+      <c r="D4" s="48">
         <v>26.655000000000001</v>
       </c>
-      <c r="E5" s="52">
-        <f t="shared" ref="E5:E22" si="2">D5-B5</f>
+      <c r="E4" s="49">
+        <f t="shared" ref="E4:E21" si="2">D4-B4</f>
         <v>-11.254999999999995</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F4" s="44">
         <f t="shared" si="0"/>
         <v>-3.4999999999999947</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H4" s="44">
         <f t="shared" si="1"/>
         <v>11.313708498984719</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A6" s="51">
+      <c r="K4" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" s="48">
         <v>17</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B5" s="48">
         <v>35.879999999999995</v>
       </c>
-      <c r="C6" s="51" t="s">
-        <v>250</v>
-      </c>
-      <c r="D6" s="51">
+      <c r="C5" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" s="48">
         <v>30.035</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E5" s="49">
         <f t="shared" si="2"/>
         <v>-5.8449999999999953</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F5" s="44">
         <f t="shared" si="0"/>
         <v>1.9100000000000055</v>
       </c>
-      <c r="H6" s="47">
+      <c r="H5" s="44">
         <f t="shared" si="1"/>
         <v>0.26609254561333895</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A7" s="51">
+      <c r="K5" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" s="48">
         <v>18</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B6" s="48">
         <v>37.299999999999997</v>
       </c>
-      <c r="C7" s="51" t="s">
-        <v>251</v>
-      </c>
-      <c r="D7" s="51">
+      <c r="C6" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="D6" s="48">
         <v>33.380000000000003</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E6" s="49">
         <f t="shared" si="2"/>
         <v>-3.9199999999999946</v>
       </c>
-      <c r="F7" s="47">
+      <c r="F6" s="44">
         <f t="shared" si="0"/>
         <v>3.8350000000000062</v>
       </c>
-      <c r="H7" s="47">
+      <c r="H6" s="44">
         <f t="shared" si="1"/>
         <v>7.0072879876781499E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A8" s="51">
+      <c r="K6" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A7" s="48">
         <v>10</v>
       </c>
-      <c r="B8" s="51">
+      <c r="B7" s="48">
         <v>40</v>
       </c>
-      <c r="C8" s="51" t="s">
-        <v>244</v>
-      </c>
-      <c r="D8" s="51">
+      <c r="C7" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="48">
         <v>31.375</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E7" s="49">
         <f t="shared" si="2"/>
         <v>-8.625</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F7" s="44">
         <f t="shared" si="0"/>
         <v>-0.86999999999999922</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H7" s="44">
         <f t="shared" si="1"/>
         <v>1.8276629004587999</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A9" s="51">
+      <c r="K7" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A8" s="48">
         <v>19</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B8" s="48">
         <v>37.825000000000003</v>
       </c>
-      <c r="C9" s="51" t="s">
-        <v>252</v>
-      </c>
-      <c r="D9" s="51">
+      <c r="C8" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="48">
         <v>33.135000000000005</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E8" s="49">
         <f t="shared" si="2"/>
         <v>-4.6899999999999977</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F8" s="44">
         <f t="shared" si="0"/>
         <v>3.0650000000000031</v>
       </c>
-      <c r="H9" s="47">
+      <c r="H8" s="44">
         <f t="shared" si="1"/>
         <v>0.11949316469921753</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A10" s="51">
+      <c r="K8" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" s="48">
         <v>16</v>
       </c>
-      <c r="B10" s="51">
+      <c r="B9" s="48">
         <v>38.760000000000005</v>
       </c>
-      <c r="C10" s="51" t="s">
-        <v>249</v>
-      </c>
-      <c r="D10" s="51">
+      <c r="C9" s="48" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="48">
         <v>33.08</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E9" s="49">
         <f t="shared" si="2"/>
         <v>-5.6800000000000068</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F9" s="44">
         <f t="shared" si="0"/>
         <v>2.074999999999994</v>
       </c>
-      <c r="H10" s="47">
+      <c r="H9" s="44">
         <f t="shared" si="1"/>
         <v>0.23733553023763082</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A11" s="51">
+      <c r="K9" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" s="48">
         <v>7</v>
       </c>
-      <c r="B11" s="53">
+      <c r="B10" s="50">
         <v>39.81</v>
       </c>
-      <c r="C11" s="51" t="s">
-        <v>241</v>
-      </c>
-      <c r="D11" s="51">
+      <c r="C10" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="48">
         <v>33.094999999999999</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E10" s="49">
         <f t="shared" si="2"/>
         <v>-6.7150000000000034</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F10" s="44">
         <f t="shared" si="0"/>
         <v>1.0399999999999974</v>
       </c>
-      <c r="H11" s="47">
+      <c r="H10" s="44">
         <f t="shared" si="1"/>
         <v>0.48632747370614371</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A12" s="51">
+      <c r="K10" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A11" s="48">
         <v>6</v>
       </c>
-      <c r="B12" s="53">
+      <c r="B11" s="50">
         <v>38.57</v>
       </c>
-      <c r="C12" s="51" t="s">
-        <v>240</v>
-      </c>
-      <c r="D12" s="51">
+      <c r="C11" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D11" s="48">
         <v>25.83</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E11" s="49">
         <f t="shared" si="2"/>
         <v>-12.740000000000002</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F11" s="44">
         <f t="shared" si="0"/>
         <v>-4.9850000000000012</v>
       </c>
-      <c r="H12" s="47">
+      <c r="H11" s="44">
         <f t="shared" si="1"/>
         <v>31.669013005286651</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A13" s="48">
+      <c r="K11" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" s="45">
         <v>1</v>
       </c>
-      <c r="B13" s="50">
+      <c r="B12" s="47">
         <v>36.049999999999997</v>
       </c>
-      <c r="C13" s="48" t="s">
-        <v>235</v>
-      </c>
-      <c r="D13" s="48">
+      <c r="C12" s="45" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" s="45">
         <v>24.73</v>
       </c>
-      <c r="E13" s="49">
+      <c r="E12" s="46">
         <f t="shared" si="2"/>
         <v>-11.319999999999997</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F12" s="44">
         <f t="shared" si="0"/>
         <v>-3.5649999999999959</v>
       </c>
-      <c r="H13" s="47">
+      <c r="H12" s="44">
         <f t="shared" si="1"/>
         <v>11.835100073990667</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A14" s="48">
+      <c r="K12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A13" s="45">
         <v>14</v>
       </c>
-      <c r="B14" s="48">
+      <c r="B13" s="45">
         <v>34.945</v>
       </c>
-      <c r="C14" s="48" t="s">
-        <v>254</v>
-      </c>
-      <c r="D14" s="48">
+      <c r="C13" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="D13" s="45">
         <v>26.134999999999998</v>
       </c>
-      <c r="E14" s="49">
+      <c r="E13" s="46">
         <f t="shared" si="2"/>
         <v>-8.8100000000000023</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F13" s="44">
         <f t="shared" si="0"/>
         <v>-1.0550000000000015</v>
       </c>
-      <c r="H14" s="47">
+      <c r="H13" s="44">
         <f t="shared" si="1"/>
         <v>2.0777182065953306</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A15" s="48">
+      <c r="K13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A14" s="45">
         <v>3</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B14" s="45">
         <v>35.06</v>
       </c>
-      <c r="C15" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="D15" s="48">
+      <c r="C14" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" s="45">
         <v>25.6</v>
       </c>
-      <c r="E15" s="49">
+      <c r="E14" s="46">
         <f t="shared" si="2"/>
         <v>-9.4600000000000009</v>
       </c>
-      <c r="F15" s="47">
+      <c r="F14" s="44">
         <f t="shared" si="0"/>
         <v>-1.7050000000000001</v>
       </c>
-      <c r="H15" s="47">
+      <c r="H14" s="44">
         <f t="shared" si="1"/>
         <v>3.2602893296105018</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A16" s="48">
-        <v>12</v>
-      </c>
-      <c r="B16" s="50">
+      <c r="K14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A15" s="45">
+        <v>12</v>
+      </c>
+      <c r="B15" s="47">
         <v>39.979999999999997</v>
       </c>
-      <c r="C16" s="48" t="s">
-        <v>246</v>
-      </c>
-      <c r="D16" s="48">
+      <c r="C15" s="45" t="s">
+        <v>243</v>
+      </c>
+      <c r="D15" s="45">
         <v>32.445</v>
       </c>
-      <c r="E16" s="49">
+      <c r="E15" s="46">
         <f t="shared" si="2"/>
         <v>-7.5349999999999966</v>
       </c>
-      <c r="F16" s="47">
+      <c r="F15" s="44">
         <f t="shared" si="0"/>
         <v>0.22000000000000419</v>
       </c>
-      <c r="H16" s="47">
+      <c r="H15" s="44">
         <f t="shared" si="1"/>
         <v>0.85856543643775129</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="48">
+      <c r="K15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A16" s="45">
         <v>8</v>
       </c>
-      <c r="B17" s="48">
+      <c r="B16" s="45">
         <v>40</v>
       </c>
-      <c r="C17" s="48" t="s">
-        <v>242</v>
-      </c>
-      <c r="D17" s="48">
+      <c r="C16" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="D16" s="45">
         <v>33.54</v>
       </c>
-      <c r="E17" s="49">
+      <c r="E16" s="46">
         <f t="shared" si="2"/>
         <v>-6.4600000000000009</v>
       </c>
-      <c r="F17" s="47">
+      <c r="F16" s="44">
         <f t="shared" si="0"/>
         <v>1.2949999999999999</v>
       </c>
-      <c r="H17" s="47">
+      <c r="H16" s="44">
         <f t="shared" si="1"/>
         <v>0.40753616620131272</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="48">
+      <c r="K16" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A17" s="45">
         <v>5</v>
       </c>
-      <c r="B18" s="48">
+      <c r="B17" s="45">
         <v>40</v>
       </c>
-      <c r="C18" s="48" t="s">
-        <v>239</v>
-      </c>
-      <c r="D18" s="48">
+      <c r="C17" s="45" t="s">
+        <v>236</v>
+      </c>
+      <c r="D17" s="45">
         <v>39.36</v>
       </c>
-      <c r="E18" s="49">
+      <c r="E17" s="46">
         <f t="shared" si="2"/>
         <v>-0.64000000000000057</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F17" s="44">
         <f t="shared" si="0"/>
         <v>7.1150000000000002</v>
       </c>
-      <c r="H18" s="47">
+      <c r="H17" s="44">
         <f t="shared" si="1"/>
         <v>7.2139243025733995E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="48">
+      <c r="K17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A18" s="45">
         <v>9</v>
       </c>
-      <c r="B19" s="48">
+      <c r="B18" s="45">
         <v>40</v>
       </c>
-      <c r="C19" s="48" t="s">
-        <v>243</v>
-      </c>
-      <c r="D19" s="48">
+      <c r="C18" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" s="45">
         <v>31.134999999999998</v>
       </c>
-      <c r="E19" s="49">
+      <c r="E18" s="46">
         <f t="shared" si="2"/>
         <v>-8.865000000000002</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F18" s="44">
         <f t="shared" si="0"/>
         <v>-1.1100000000000012</v>
       </c>
-      <c r="H19" s="47">
+      <c r="H18" s="44">
         <f t="shared" si="1"/>
         <v>2.1584564730088562</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="48">
+      <c r="K18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A19" s="45">
         <v>20</v>
       </c>
-      <c r="B20" s="48">
+      <c r="B19" s="45">
         <v>39.564999999999998</v>
       </c>
-      <c r="C20" s="48" t="s">
-        <v>253</v>
-      </c>
-      <c r="D20" s="48">
+      <c r="C19" s="45" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" s="45">
         <v>34.96</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E19" s="46">
         <f t="shared" si="2"/>
         <v>-4.6049999999999969</v>
       </c>
-      <c r="F20" s="47">
+      <c r="F19" s="44">
         <f t="shared" si="0"/>
         <v>3.1500000000000039</v>
       </c>
-      <c r="H20" s="47">
+      <c r="H19" s="44">
         <f t="shared" si="1"/>
         <v>0.11265630782635351</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="48">
-        <v>13</v>
-      </c>
-      <c r="B21" s="48">
+      <c r="K19" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A20" s="45">
+        <v>13</v>
+      </c>
+      <c r="B20" s="45">
         <v>40</v>
       </c>
-      <c r="C21" s="48" t="s">
-        <v>247</v>
-      </c>
-      <c r="D21" s="48">
+      <c r="C20" s="45" t="s">
+        <v>244</v>
+      </c>
+      <c r="D20" s="45">
         <v>33.634999999999998</v>
       </c>
-      <c r="E21" s="49">
+      <c r="E20" s="46">
         <f t="shared" si="2"/>
         <v>-6.365000000000002</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F20" s="44">
         <f t="shared" si="0"/>
         <v>1.3899999999999988</v>
       </c>
-      <c r="H21" s="47">
+      <c r="H20" s="44">
         <f t="shared" si="1"/>
         <v>0.38156480224014017</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="48">
+      <c r="K20" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A21" s="45">
         <v>15</v>
       </c>
-      <c r="B22" s="48">
+      <c r="B21" s="45">
         <v>36.655000000000001</v>
       </c>
-      <c r="C22" s="48" t="s">
-        <v>248</v>
-      </c>
-      <c r="D22" s="48">
+      <c r="C21" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="D21" s="45">
         <v>31.765000000000001</v>
       </c>
-      <c r="E22" s="49">
+      <c r="E21" s="46">
         <f t="shared" si="2"/>
         <v>-4.8900000000000006</v>
       </c>
-      <c r="F22" s="47">
+      <c r="F21" s="44">
         <f t="shared" si="0"/>
         <v>2.8650000000000002</v>
       </c>
-      <c r="H22" s="47">
+      <c r="H21" s="44">
         <f t="shared" si="1"/>
         <v>0.13726160172338123</v>
       </c>
+      <c r="K21" t="s">
+        <v>259</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D41" xr:uid="{4D366DB0-ADA9-7F47-A64B-307E5A959B55}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G22">
-    <sortCondition ref="C3:C22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+    <sortCondition ref="C2:C21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -42495,7 +42546,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="54" t="s">
         <v>215</v>
       </c>
       <c r="B2" s="31" t="s">
@@ -42539,7 +42590,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A3" s="45"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="33" t="s">
         <v>4</v>
       </c>
@@ -42557,7 +42608,7 @@
       <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A4" s="46"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="35" t="s">
         <v>216</v>
       </c>
@@ -42589,7 +42640,7 @@
       <c r="N4" s="36"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="54" t="s">
         <v>217</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -42633,7 +42684,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A6" s="45"/>
+      <c r="A6" s="55"/>
       <c r="B6" s="33" t="s">
         <v>4</v>
       </c>
@@ -42651,7 +42702,7 @@
       <c r="N6" s="34"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A7" s="46"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="35" t="s">
         <v>216</v>
       </c>
@@ -42681,7 +42732,7 @@
       <c r="N7" s="36"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="54" t="s">
         <v>218</v>
       </c>
       <c r="B8" s="31" t="s">
@@ -42725,7 +42776,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A9" s="45"/>
+      <c r="A9" s="55"/>
       <c r="B9" s="33" t="s">
         <v>4</v>
       </c>
@@ -42743,7 +42794,7 @@
       <c r="N9" s="34"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A10" s="46"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="35" t="s">
         <v>216</v>
       </c>
@@ -42781,7 +42832,7 @@
       <c r="N10" s="36"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="54" t="s">
         <v>219</v>
       </c>
       <c r="B11" s="31" t="s">
@@ -42825,7 +42876,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A12" s="45"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="33" t="s">
         <v>4</v>
       </c>
@@ -42843,7 +42894,7 @@
       <c r="N12" s="34"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A13" s="46"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="35" t="s">
         <v>216</v>
       </c>
@@ -42879,7 +42930,7 @@
       <c r="N13" s="36"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="54" t="s">
         <v>220</v>
       </c>
       <c r="B14" s="31" t="s">
@@ -42923,7 +42974,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A15" s="45"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="33" t="s">
         <v>4</v>
       </c>
@@ -42941,7 +42992,7 @@
       <c r="N15" s="34"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A16" s="46"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="35" t="s">
         <v>216</v>
       </c>
@@ -42975,7 +43026,7 @@
       <c r="N16" s="36"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="54" t="s">
         <v>221</v>
       </c>
       <c r="B17" s="31" t="s">
@@ -43019,7 +43070,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A18" s="45"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="33" t="s">
         <v>4</v>
       </c>
@@ -43037,7 +43088,7 @@
       <c r="N18" s="34"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A19" s="46"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="35" t="s">
         <v>216</v>
       </c>
@@ -43073,7 +43124,7 @@
       <c r="N19" s="36"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="54" t="s">
         <v>222</v>
       </c>
       <c r="B20" s="31" t="s">
@@ -43117,7 +43168,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A21" s="45"/>
+      <c r="A21" s="55"/>
       <c r="B21" s="33" t="s">
         <v>4</v>
       </c>
@@ -43135,7 +43186,7 @@
       <c r="N21" s="34"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A22" s="46"/>
+      <c r="A22" s="56"/>
       <c r="B22" s="35" t="s">
         <v>216</v>
       </c>
@@ -43167,7 +43218,7 @@
       <c r="N22" s="36"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="54" t="s">
         <v>223</v>
       </c>
       <c r="B23" s="31" t="s">
@@ -43211,7 +43262,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A24" s="45"/>
+      <c r="A24" s="55"/>
       <c r="B24" s="33" t="s">
         <v>4</v>
       </c>
@@ -43229,7 +43280,7 @@
       <c r="N24" s="34"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A25" s="46"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="35" t="s">
         <v>216</v>
       </c>

</xml_diff>